<commit_message>
them hd add anh vao file excel
</commit_message>
<xml_diff>
--- a/public/ex_files/example_questions_import.xlsx
+++ b/public/ex_files/example_questions_import.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Quang Vinh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C83C7B-67D7-4BC8-9884-E8166664F27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3BE282-8F45-4A6F-A202-9AE69956C2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Câu hỏi" sheetId="1" r:id="rId1"/>
     <sheet name="Ảnh" sheetId="3" r:id="rId2"/>
+    <sheet name="Hướng dẫn chèn ảnh" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" forceFullCalc="1"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Đáp án đúng</t>
   </si>
@@ -165,13 +166,80 @@
   </si>
   <si>
     <t>Nguyễn Huệ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>[Sheet Câu hỏi]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Trong câu hỏi chứa ảnh, tại cột "Image Code", nhập mã ảnh theo cú pháp anh* với * là số tự nhiên
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Lưu ý: 
+- Mã ảnh không được phép trùng
+- Mã ảnh phải cùng hàng với hàng chứa dữ liệu của cột "Title Origin"
+- VD: [anh1], [anh2], [anh3], …</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>[Sheet Ảnh]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Điền mã ảnh, chèn ảnh theo đúng thứ tự</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+- VD: anh1, anh2, anh3, …</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -241,6 +309,19 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -264,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -281,6 +362,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -444,6 +531,111 @@
         <a:xfrm>
           <a:off x="1614744" y="2964180"/>
           <a:ext cx="2058096" cy="1287780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5219700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5076714</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>2705100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FED570CC-EE8D-3C1D-8751-43611BC4B4CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5219700" y="0"/>
+          <a:ext cx="5091954" cy="2705100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5059680</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>13335</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03478E01-95A7-0306-E1AF-93A8E0A6B019}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5234940" y="2621280"/>
+          <a:ext cx="5059680" cy="2687955"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -745,8 +937,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1010,4 +1202,34 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B845293-1130-4D98-86E7-137D001353B4}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="76.33203125" customWidth="1"/>
+    <col min="2" max="2" width="74.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="217.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="210.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>